<commit_message>
formated a bit szavazasExcel
</commit_message>
<xml_diff>
--- a/szavazás excel alap.xlsx
+++ b/szavazás excel alap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>UML</t>
   </si>
@@ -60,13 +60,16 @@
   </si>
   <si>
     <t>domiterpelda.doc</t>
+  </si>
+  <si>
+    <t>csapatvezető</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,16 +78,45 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -92,14 +124,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Címsor 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -378,78 +443,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>